<commit_message>
final re-run including fig: unmet social support
</commit_message>
<xml_diff>
--- a/data/raw/20250918_Inclusion and exclusion.xlsx
+++ b/data/raw/20250918_Inclusion and exclusion.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kuleuven-my.sharepoint.com/personal/vicky_steyfkens_kuleuven_be/Documents/1. NEED Project/2. Analyse en resultaten/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\0055_Projects\FAR\BA25_Claessens_KCETables\NEED-GQ\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BA1CD43D-CD71-674A-8A97-84A17914F95F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB7A7C30-5E0E-434B-89C5-F6EBBDFA911C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-5240" yWindow="-21100" windowWidth="38400" windowHeight="19640" activeTab="2" xr2:uid="{7FCD9C44-F21D-A641-9725-E69AD16AD229}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{7FCD9C44-F21D-A641-9725-E69AD16AD229}"/>
   </bookViews>
   <sheets>
     <sheet name="To be excluded" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="24">
   <si>
     <t>ID's that needs to be exluded from the data:</t>
   </si>
@@ -101,13 +101,22 @@
   </si>
   <si>
     <t>Schizophrénia</t>
+  </si>
+  <si>
+    <t>Associated variable</t>
+  </si>
+  <si>
+    <t>DSD1_A1</t>
+  </si>
+  <si>
+    <t>DSD1_A9</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -141,6 +150,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -170,7 +185,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -186,7 +201,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -508,18 +523,18 @@
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.33203125" customWidth="1"/>
-    <col min="3" max="3" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.375" customWidth="1"/>
+    <col min="3" max="3" width="27.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -530,7 +545,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>4</v>
       </c>
@@ -541,7 +556,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>11</v>
       </c>
@@ -552,7 +567,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>28</v>
       </c>
@@ -563,7 +578,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>29</v>
       </c>
@@ -574,7 +589,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>37</v>
       </c>
@@ -585,7 +600,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>56</v>
       </c>
@@ -596,7 +611,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>57</v>
       </c>
@@ -607,7 +622,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>65</v>
       </c>
@@ -618,7 +633,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>77</v>
       </c>
@@ -629,7 +644,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>78</v>
       </c>
@@ -640,7 +655,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>166</v>
       </c>
@@ -651,7 +666,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>168</v>
       </c>
@@ -662,7 +677,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>203</v>
       </c>
@@ -673,7 +688,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>229</v>
       </c>
@@ -684,7 +699,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>250</v>
       </c>
@@ -695,7 +710,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>266</v>
       </c>
@@ -706,7 +721,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>277</v>
       </c>
@@ -717,7 +732,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>278</v>
       </c>
@@ -728,7 +743,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>283</v>
       </c>
@@ -739,7 +754,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>285</v>
       </c>
@@ -750,7 +765,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>292</v>
       </c>
@@ -761,7 +776,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>297</v>
       </c>
@@ -772,7 +787,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>300</v>
       </c>
@@ -783,7 +798,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>303</v>
       </c>
@@ -794,7 +809,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>304</v>
       </c>
@@ -805,7 +820,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>315</v>
       </c>
@@ -816,7 +831,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>316</v>
       </c>
@@ -827,7 +842,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>324</v>
       </c>
@@ -838,7 +853,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>330</v>
       </c>
@@ -849,7 +864,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>332</v>
       </c>
@@ -860,7 +875,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>342</v>
       </c>
@@ -871,7 +886,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>360</v>
       </c>
@@ -882,7 +897,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>361</v>
       </c>
@@ -893,7 +908,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>380</v>
       </c>
@@ -904,7 +919,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>388</v>
       </c>
@@ -924,21 +939,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F6540F4-C7F6-D142-A31A-62D6C7E7133D}">
   <dimension ref="A1:B26"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="A26" sqref="A3:A26"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -946,7 +961,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>52</v>
       </c>
@@ -954,7 +969,7 @@
         <v>1251475078</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>58</v>
       </c>
@@ -962,7 +977,7 @@
         <v>1144774775</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>70</v>
       </c>
@@ -970,7 +985,7 @@
         <v>495996092</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>88</v>
       </c>
@@ -978,7 +993,7 @@
         <v>2091803638</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>103</v>
       </c>
@@ -986,7 +1001,7 @@
         <v>1890078034</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>134</v>
       </c>
@@ -994,7 +1009,7 @@
         <v>1040814706</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>200</v>
       </c>
@@ -1002,7 +1017,7 @@
         <v>2063281544</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>219</v>
       </c>
@@ -1010,7 +1025,7 @@
         <v>2015753488</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>220</v>
       </c>
@@ -1018,7 +1033,7 @@
         <v>2100070896</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>222</v>
       </c>
@@ -1026,7 +1041,7 @@
         <v>1758525081</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>223</v>
       </c>
@@ -1034,7 +1049,7 @@
         <v>1133656069</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>231</v>
       </c>
@@ -1042,7 +1057,7 @@
         <v>1054563248</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>236</v>
       </c>
@@ -1050,7 +1065,7 @@
         <v>741313898</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>251</v>
       </c>
@@ -1058,7 +1073,7 @@
         <v>38478309</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>262</v>
       </c>
@@ -1066,7 +1081,7 @@
         <v>1963898415</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>275</v>
       </c>
@@ -1074,7 +1089,7 @@
         <v>1691898288</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>291</v>
       </c>
@@ -1082,7 +1097,7 @@
         <v>1064923690</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>310</v>
       </c>
@@ -1090,7 +1105,7 @@
         <v>909561869</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>319</v>
       </c>
@@ -1098,7 +1113,7 @@
         <v>556543743</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>338</v>
       </c>
@@ -1106,7 +1121,7 @@
         <v>1891517157</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>350</v>
       </c>
@@ -1114,7 +1129,7 @@
         <v>1892864650</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>351</v>
       </c>
@@ -1122,7 +1137,7 @@
         <v>636124101</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>353</v>
       </c>
@@ -1130,7 +1145,7 @@
         <v>1253213637</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>369</v>
       </c>
@@ -1145,24 +1160,24 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{968891BA-9C43-9540-9A36-6CCBC6E08F06}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="179" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.83203125" customWidth="1"/>
+    <col min="2" max="2" width="14.875" customWidth="1"/>
     <col min="3" max="3" width="29" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
@@ -1172,8 +1187,11 @@
       <c r="C2" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>21</v>
       </c>
@@ -1183,8 +1201,11 @@
       <c r="C3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>27</v>
       </c>
@@ -1194,8 +1215,11 @@
       <c r="C4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>49</v>
       </c>
@@ -1205,8 +1229,11 @@
       <c r="C5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>58</v>
       </c>
@@ -1216,8 +1243,11 @@
       <c r="C6" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>80</v>
       </c>
@@ -1227,8 +1257,11 @@
       <c r="C7" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>146</v>
       </c>
@@ -1238,8 +1271,11 @@
       <c r="C8" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>371</v>
       </c>
@@ -1249,8 +1285,11 @@
       <c r="C9" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>390</v>
       </c>
@@ -1260,8 +1299,12 @@
       <c r="C10" t="s">
         <v>19</v>
       </c>
+      <c r="D10" t="s">
+        <v>23</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>